<commit_message>
Fix adversary defaults to match comprehensive tier/type table
- Updated all adversary type defaults to match exact values from comprehensive table
- Fixed Bruiser, Horde, Leader, Ranged, Skulk, Solo, Support, and Social values
- Corrected difficulty, thresholds, HP, stress, attack, and damage expressions
- All custom adversary creation now uses accurate SRD-based defaults
- Incremented version to 0.4.2
</commit_message>
<xml_diff>
--- a/src/data/daggerheart_math_condensed_with_counts.xlsx
+++ b/src/data/daggerheart_math_condensed_with_counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a0410b60afd4b9f4/Coding/daggerheart app/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1040" documentId="8_{6B9BB478-F258-1349-B169-2A87E8E1C059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1CDCF97-C783-3F4F-97AB-7908DB226E18}"/>
+  <xr:revisionPtr revIDLastSave="1053" documentId="8_{6B9BB478-F258-1349-B169-2A87E8E1C059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C959155F-C8F2-474B-8A3F-707515C907F2}"/>
   <bookViews>
     <workbookView xWindow="3280" yWindow="3100" windowWidth="27640" windowHeight="16940" xr2:uid="{B82AAEBC-F5B2-A24D-9A24-328C196118E1}"/>
   </bookViews>
@@ -882,29 +882,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DDD272C-E2A1-4F4A-9638-CD8320E8F630}" name="Table1" displayName="Table1" ref="A1:Q51" totalsRowShown="0">
-  <autoFilter ref="A1:Q51" xr:uid="{8DDD272C-E2A1-4F4A-9638-CD8320E8F630}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-        <filter val="2"/>
-        <filter val="3"/>
-        <filter val="4"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Bruiser"/>
-        <filter val="Horde"/>
-        <filter val="Leader"/>
-        <filter val="Minion"/>
-        <filter val="Ranged"/>
-        <filter val="Skulk"/>
-        <filter val="Solo"/>
-        <filter val="Standard"/>
-        <filter val="Support"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q51" xr:uid="{8DDD272C-E2A1-4F4A-9638-CD8320E8F630}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q51">
     <sortCondition ref="B1:B51"/>
   </sortState>
@@ -1255,10 +1233,10 @@
   <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" sqref="A1:K50"/>
+      <selection pane="bottomRight" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,7 +1244,8 @@
     <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" customWidth="1"/>
     <col min="5" max="6" width="13" customWidth="1"/>
-    <col min="10" max="14" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="17.5" hidden="1" customWidth="1"/>
+    <col min="11" max="14" width="17.5" customWidth="1"/>
     <col min="15" max="15" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1531,7 +1510,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1763,7 +1742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -1995,7 +1974,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -2227,7 +2206,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2434,7 +2413,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -2666,7 +2645,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2898,7 +2877,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -2910,7 +2889,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2959,7 +2938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
@@ -3008,7 +2987,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -3057,7 +3036,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3106,7 +3085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -3348,7 +3327,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3583,7 +3562,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>82</v>
       </c>

</xml_diff>